<commit_message>
update behavior when close window
</commit_message>
<xml_diff>
--- a/01_概要設計書/概要設計書.xlsx
+++ b/01_概要設計書/概要設計書.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="19395" windowHeight="7605" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="19395" windowHeight="7605"/>
   </bookViews>
   <sheets>
     <sheet name="概要設計" sheetId="1" r:id="rId1"/>
@@ -1075,31 +1075,22 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>更新がDBに反映されていない場合、警告メッセージを表示する。</t>
-    <rPh sb="0" eb="2">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ハンエイ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ケイコク</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>画面を閉じる</t>
     <rPh sb="0" eb="2">
       <t>ガメン</t>
     </rPh>
     <rPh sb="3" eb="4">
       <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB未反映分はリセットされる。</t>
+    <rPh sb="2" eb="5">
+      <t>ミハンエイ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ブン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1301,31 +1292,31 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5579,7 +5570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M129"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
@@ -5627,79 +5618,79 @@
     </row>
     <row r="11" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="9"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="10"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6">
         <v>9.4</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="10"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6">
         <v>2.5</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="10"/>
     </row>
     <row r="16" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="11"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B19" s="1">
@@ -6124,13 +6115,13 @@
         <v>78</v>
       </c>
       <c r="E127" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="128" spans="4:5" x14ac:dyDescent="0.15">
       <c r="D128" s="2"/>
       <c r="E128" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.15">
@@ -6138,16 +6129,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="C16:G16"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6159,7 +6150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add link that to menu
</commit_message>
<xml_diff>
--- a/01_概要設計書/概要設計書.xlsx
+++ b/01_概要設計書/概要設計書.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="90">
   <si>
     <t>ツール概要</t>
     <rPh sb="3" eb="5">
@@ -1091,6 +1091,16 @@
     </rPh>
     <rPh sb="5" eb="6">
       <t>ブン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メニューへ画面遷移できるようになる。</t>
+    <rPh sb="5" eb="7">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>センイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1292,31 +1302,31 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2512,6 +2522,56 @@
           <a:ext cx="1663555" cy="2"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>74957</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>17816</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>148881</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="カギ線コネクタ 10"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="3"/>
+          <a:endCxn id="27" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4354166" y="3918087"/>
+          <a:ext cx="873411" cy="2509011"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
@@ -5254,6 +5314,67 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>638174</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="正方形/長方形 69"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2495549" y="8667750"/>
+          <a:ext cx="885825" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>メニューへ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5568,10 +5689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M129"/>
+  <dimension ref="B2:M130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.375" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5618,79 +5739,79 @@
     </row>
     <row r="11" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="9"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="10"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5">
         <v>9.4</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="10"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5">
         <v>2.5</v>
       </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="10"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="11"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="8"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B19" s="1">
@@ -5768,158 +5889,156 @@
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C54" s="2"/>
+      <c r="D54" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C55" s="2"/>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C57" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="D57" t="s">
+    <row r="58" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="D58" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C58" s="2"/>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C59" s="2"/>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="D60" s="2" t="s">
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="D61" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E61" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="E61" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.15">
       <c r="E62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.15">
       <c r="E63" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="E64" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="D66" t="s">
+    <row r="67" spans="3:13" x14ac:dyDescent="0.15">
+      <c r="D67" t="s">
         <v>39</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E67" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="E67" t="s">
+    <row r="68" spans="3:13" x14ac:dyDescent="0.15">
+      <c r="E68" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C70" s="2" t="s">
+    <row r="71" spans="3:13" x14ac:dyDescent="0.15">
+      <c r="C71" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="D71" t="s">
+    <row r="72" spans="3:13" x14ac:dyDescent="0.15">
+      <c r="D72" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="D74" s="2" t="s">
+    <row r="75" spans="3:13" x14ac:dyDescent="0.15">
+      <c r="D75" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E75" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="E75" t="s">
+    <row r="76" spans="3:13" x14ac:dyDescent="0.15">
+      <c r="E76" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="76" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="F76" t="s">
-        <v>47</v>
-      </c>
-      <c r="I76" t="s">
-        <v>51</v>
-      </c>
-      <c r="M76" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="77" spans="3:13" x14ac:dyDescent="0.15">
       <c r="F77" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I77" t="s">
         <v>51</v>
       </c>
+      <c r="M77" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="78" spans="3:13" x14ac:dyDescent="0.15">
       <c r="F78" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="I78" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="3:13" x14ac:dyDescent="0.15">
       <c r="F79" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="I79" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="3:13" x14ac:dyDescent="0.15">
       <c r="F80" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I80" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="4:9" x14ac:dyDescent="0.15">
-      <c r="D83" s="2" t="s">
+    <row r="81" spans="4:9" x14ac:dyDescent="0.15">
+      <c r="F81" t="s">
+        <v>50</v>
+      </c>
+      <c r="I81" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="84" spans="4:9" x14ac:dyDescent="0.15">
+      <c r="D84" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E84" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="4:9" x14ac:dyDescent="0.15">
-      <c r="E84" t="s">
+    <row r="85" spans="4:9" x14ac:dyDescent="0.15">
+      <c r="E85" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="85" spans="4:9" x14ac:dyDescent="0.15">
-      <c r="F85" t="s">
-        <v>47</v>
-      </c>
-      <c r="I85" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="86" spans="4:9" x14ac:dyDescent="0.15">
       <c r="F86" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I86" t="s">
         <v>51</v>
@@ -5927,39 +6046,39 @@
     </row>
     <row r="87" spans="4:9" x14ac:dyDescent="0.15">
       <c r="F87" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="I87" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="4:9" x14ac:dyDescent="0.15">
       <c r="F88" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="I88" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="89" spans="4:9" x14ac:dyDescent="0.15">
       <c r="F89" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I89" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="4:9" x14ac:dyDescent="0.15">
-      <c r="E91" t="s">
+    <row r="90" spans="4:9" x14ac:dyDescent="0.15">
+      <c r="F90" t="s">
+        <v>50</v>
+      </c>
+      <c r="I90" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92" spans="4:9" x14ac:dyDescent="0.15">
+      <c r="E92" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="92" spans="4:9" x14ac:dyDescent="0.15">
-      <c r="F92" t="s">
-        <v>64</v>
-      </c>
-      <c r="G92" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="93" spans="4:9" x14ac:dyDescent="0.15">
@@ -5967,7 +6086,7 @@
         <v>64</v>
       </c>
       <c r="G93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="94" spans="4:9" x14ac:dyDescent="0.15">
@@ -5975,7 +6094,7 @@
         <v>64</v>
       </c>
       <c r="G94" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="95" spans="4:9" x14ac:dyDescent="0.15">
@@ -5983,7 +6102,7 @@
         <v>64</v>
       </c>
       <c r="G95" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="96" spans="4:9" x14ac:dyDescent="0.15">
@@ -5991,154 +6110,162 @@
         <v>64</v>
       </c>
       <c r="G96" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="97" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="F97" t="s">
+        <v>64</v>
+      </c>
+      <c r="G97" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="D99" s="2" t="s">
+    <row r="100" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="D100" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="E100" t="s">
+    <row r="101" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="E101" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="D103" s="2" t="s">
+    <row r="104" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="D104" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E104" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="E104" t="s">
+    <row r="105" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="E105" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="107" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="D107" s="2" t="s">
+    <row r="108" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="D108" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E108" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="D108" s="2"/>
-      <c r="E108" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="109" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="109" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D109" s="2"/>
       <c r="E109" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="110" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="D110" s="2"/>
+      <c r="E110" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="D110" s="2"/>
-    </row>
-    <row r="111" spans="4:5" x14ac:dyDescent="0.15">
+    <row r="111" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="D112" s="2" t="s">
+    <row r="112" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D113" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E113" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="113" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="E113" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="114" spans="4:5" x14ac:dyDescent="0.15">
       <c r="E114" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="115" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="E115" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="116" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="D116" s="2" t="s">
+    <row r="117" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D117" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E117" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="117" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="E117" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="118" spans="4:5" x14ac:dyDescent="0.15">
       <c r="E118" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="119" spans="4:5" x14ac:dyDescent="0.15">
       <c r="E119" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="E120" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="121" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="D121" s="2" t="s">
+    <row r="122" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D122" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E122" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="122" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="E122" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="123" spans="4:5" x14ac:dyDescent="0.15">
       <c r="E123" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="124" spans="4:5" x14ac:dyDescent="0.15">
       <c r="E124" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="125" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="E125" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="127" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="D127" s="2" t="s">
+    <row r="128" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D128" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E127" t="s">
+      <c r="E128" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="128" spans="4:5" x14ac:dyDescent="0.15">
-      <c r="D128" s="2"/>
-      <c r="E128" t="s">
+    <row r="129" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D129" s="2"/>
+      <c r="E129" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D129" s="2"/>
+    <row r="130" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D130" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
     <mergeCell ref="H12:K12"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="H14:K14"/>
     <mergeCell ref="H15:K15"/>
     <mergeCell ref="H16:K16"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6150,8 +6277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>